<commit_message>
CertificateBill and TaipowerBill Done
</commit_message>
<xml_diff>
--- a/ExcelTester/bin/Debug/net8.0-windows/Templates/台電轉供費用_請付款單範本1.xlsx
+++ b/ExcelTester/bin/Debug/net8.0-windows/Templates/台電轉供費用_請付款單範本1.xlsx
@@ -301,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <r>
       <rPr>
@@ -513,13 +513,13 @@
     </r>
   </si>
   <si>
-    <t>114/03/18</t>
+    <t>114/10/15</t>
   </si>
   <si>
     <t>事由：</t>
   </si>
   <si>
-    <t>繳納 108/03 轉供費用</t>
+    <t>繳納 108/06 轉供費用</t>
   </si>
   <si>
     <r>
@@ -732,8 +732,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">1、繳納 108/03 台電轉供費用，總計 NT$8,773 (含稅)，詳見清單。
-</t>
+    <t>1、繳納 108/06 台電轉供費用，總計 NT$167,974 (含稅)，詳見清單。</t>
   </si>
   <si>
     <t>2、匯款資料</t>
@@ -748,7 +747,7 @@
     <t xml:space="preserve">  帳號：詳見公用槽之台電轉供輸電費繳費單</t>
   </si>
   <si>
-    <t>3、請財務部安排於 114/04/24 前繳納</t>
+    <t>3、請財務部安排於 114/09/07 前繳納</t>
   </si>
   <si>
     <r>
@@ -842,12 +841,6 @@
     <t>NTD</t>
   </si>
   <si>
-    <t>Davis, Schulist and Pfannerstill</t>
-  </si>
-  <si>
-    <t>Nicolas, Haag and Schowalter</t>
-  </si>
-  <si>
     <t xml:space="preserve">請
 款</t>
   </si>
@@ -915,13 +908,49 @@
     <t>轉供輸電費(元)-含稅</t>
   </si>
   <si>
-    <t>b006d8de-4a8e-4a55-88cd-3f3099c554d9</t>
-  </si>
-  <si>
-    <t>58e020a7-98bc-4bc7-97b8-446b778e1590</t>
-  </si>
-  <si>
-    <t>ExcelTester.Classes.ExcelColumnTaipowerBillItem</t>
+    <t>08qhbhrgvt</t>
+  </si>
+  <si>
+    <t>Lubowitz and Sons</t>
+  </si>
+  <si>
+    <t>Ilene Heller</t>
+  </si>
+  <si>
+    <t>ohf77vz1nj</t>
+  </si>
+  <si>
+    <t>Stiedemann - Friesen</t>
+  </si>
+  <si>
+    <t>Colten Hegmann</t>
+  </si>
+  <si>
+    <t>osaeq8s0j6</t>
+  </si>
+  <si>
+    <t>Bernier, Greenholt and Lakin</t>
+  </si>
+  <si>
+    <t>Jonas Ankunding</t>
+  </si>
+  <si>
+    <t>bb8r6xgl6b</t>
+  </si>
+  <si>
+    <t>Hartmann, Fay and Leuschke</t>
+  </si>
+  <si>
+    <t>Aisha Blick</t>
+  </si>
+  <si>
+    <t>btzrm4gama</t>
+  </si>
+  <si>
+    <t>Ward - Yundt</t>
+  </si>
+  <si>
+    <t>Erica Feest</t>
   </si>
   <si>
     <t>總計金額</t>
@@ -1327,7 +1356,7 @@
     <numFmt numFmtId="177" formatCode="#,##0_ "/>
     <numFmt numFmtId="178" formatCode="[$-404]e/m/d;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -1421,8 +1450,13 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="標楷體"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1447,8 +1481,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="49">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1991,6 +2030,27 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1998,42 +2058,30 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -2044,7 +2092,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2237,9 +2285,6 @@
     <xf numFmtId="0" fontId="15" applyFont="1" fillId="2" applyFill="1" borderId="29" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" fontId="15" applyFont="1" fillId="2" applyFill="1" borderId="43" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" fontId="15" applyFont="1" fillId="2" applyFill="1" borderId="44" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="45" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" borderId="14" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2409,23 +2454,39 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="178" applyNumberFormat="1" fontId="7" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="178" applyNumberFormat="1" fontId="16" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="3" applyBorder="1" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="48" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" borderId="48" applyBorder="1" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="46" applyBorder="1" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="45" applyBorder="1" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="45" applyBorder="1" xfId="2"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="46" applyBorder="1" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="47" applyBorder="1" xfId="2"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="45" applyBorder="1" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="47" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="48" applyBorder="1" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="46" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="12" applyBorder="1" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="12" applyBorder="1" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="12" applyBorder="1" xfId="2"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="13" applyBorder="1" xfId="2"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="49" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="50" applyBorder="1" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="50" applyBorder="1" xfId="0"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="5" applyFill="1" borderId="51" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" fontId="15" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="46" applyBorder="1" xfId="2"/>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="14" applyFont="1" fillId="4" applyFill="1" borderId="47" applyBorder="1" xfId="2"/>
-    <xf numFmtId="3" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" applyNumberFormat="1" fontId="15" applyFont="1" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -5201,7 +5262,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:I6"/>
@@ -5227,40 +5288,40 @@
   </cols>
   <sheetData>
     <row r="1" ht="27.5">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
     </row>
     <row r="2" ht="27.5">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" ht="17.15" customHeight="1" s="3" customFormat="1">
       <c r="A3" s="14"/>
@@ -5290,58 +5351,58 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="126" t="s">
+      <c r="N4" s="125" t="s">
         <v>5</v>
       </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" ht="25.4" customHeight="1">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="96" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="100" t="s">
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103" t="s">
+      <c r="K5" s="100"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="105"/>
+      <c r="N5" s="104"/>
     </row>
     <row r="6" ht="25.4" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="99"/>
-      <c r="J6" s="107" t="s">
+      <c r="A6" s="93"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="108"/>
-      <c r="L6" s="109"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="106"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="105"/>
     </row>
     <row r="7" ht="30" customHeight="1">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
         <v>12</v>
@@ -5366,10 +5427,10 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" ht="21.5">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="72"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -5385,38 +5446,38 @@
     </row>
     <row r="9" ht="36" customHeight="1" s="14" customFormat="1">
       <c r="A9" s="54"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="78"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="77"/>
     </row>
     <row r="10" ht="24.9" customHeight="1" s="14" customFormat="1">
       <c r="A10" s="54"/>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
       <c r="N10" s="61"/>
     </row>
     <row r="11" ht="24.9" customHeight="1" s="14" customFormat="1">
@@ -5447,20 +5508,20 @@
     </row>
     <row r="14" ht="24.9" customHeight="1" s="14" customFormat="1">
       <c r="A14" s="54"/>
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="78"/>
       <c r="N14" s="61"/>
     </row>
     <row r="15" ht="20.25" customHeight="1" s="3" customFormat="1">
@@ -5475,13 +5536,13 @@
       </c>
     </row>
     <row r="16" ht="24.9" customHeight="1" s="18" customFormat="1">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="83"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="84"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
       <c r="F16" s="35" t="s">
         <v>28</v>
       </c>
@@ -5491,14 +5552,14 @@
       <c r="H16" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="80" t="s">
+      <c r="I16" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="81"/>
-      <c r="K16" s="85" t="s">
+      <c r="J16" s="80"/>
+      <c r="K16" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="84"/>
+      <c r="L16" s="83"/>
       <c r="M16" s="40" t="s">
         <v>33</v>
       </c>
@@ -5508,89 +5569,63 @@
     </row>
     <row r="17" ht="29.4" customHeight="1" s="8" customFormat="1">
       <c r="A17" s="55"/>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="86"/>
       <c r="F17" s="31" t="s">
         <v>36</v>
       </c>
       <c r="G17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="48"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="89"/>
+      <c r="H17" s="48">
+        <f>清單!E7</f>
+      </c>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="87"/>
+      <c r="L17" s="88"/>
       <c r="M17" s="49"/>
       <c r="N17" s="50"/>
     </row>
-    <row r="18">
-      <c r="B18" s="1" t="s">
+    <row r="18" ht="68.4" customHeight="1" s="8" customFormat="1">
+      <c r="A18" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="127" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="128">
-        <v>8773</v>
-      </c>
+      <c r="B18" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="59"/>
+      <c r="H18" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" s="26"/>
     </row>
-    <row r="19">
-      <c r="B19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="127" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="128">
-        <v>32974</v>
-      </c>
-    </row>
-    <row r="20" ht="68.4" customHeight="1" s="8" customFormat="1">
-      <c r="A20" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="59"/>
-      <c r="H20" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="25" t="s">
+    <row r="19" ht="24.75" customHeight="1">
+      <c r="A19" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="N20" s="26"/>
-    </row>
-    <row r="21" ht="24.75" customHeight="1">
-      <c r="A21" s="13" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -5614,8 +5649,6 @@
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLinesSet="0"/>
@@ -5631,7 +5664,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -5648,59 +5681,121 @@
   <sheetData>
     <row r="1" ht="16.5">
       <c r="A1" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="D1" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="E1" s="67" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="67" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" ht="16">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="135" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="129">
-        <v>2019</v>
-      </c>
-      <c r="C2" s="130">
-        <v>3</v>
-      </c>
-      <c r="D2" s="132">
-        <v>45771.94952552083</v>
-      </c>
-      <c r="E2" s="133">
-        <v>45734.22223630787</v>
-      </c>
-      <c r="F2" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>56</v>
+      <c r="D2" s="138">
+        <v>27212.8</v>
+      </c>
+      <c r="E2" s="139">
+        <v>34016</v>
       </c>
     </row>
     <row r="3" ht="16">
       <c r="A3" s="131" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="129" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="134">
-        <f>SUM(D2:D2)</f>
-      </c>
-      <c r="E3" s="134">
-        <f>SUM(E2:E2)</f>
+      <c r="D3" s="130">
+        <v>27046.4</v>
+      </c>
+      <c r="E3" s="132">
+        <v>33808</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="131" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="129" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="133">
+        <v>6547.2</v>
+      </c>
+      <c r="E4" s="134">
+        <v>8184</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="129" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="129" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="133">
+        <v>38400.8</v>
+      </c>
+      <c r="E5" s="134">
+        <v>48001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="140" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="141" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="141" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="142">
+        <v>35172</v>
+      </c>
+      <c r="E6" s="143">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="144" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="144"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="145">
+        <f>SUM(D2:D6)</f>
+      </c>
+      <c r="E7" s="145">
+        <f>SUM(E2:E6)</f>
       </c>
     </row>
     <row r="8">
-      <c r="E8" s="125"/>
+      <c r="E8" s="124"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -5741,40 +5836,40 @@
   </cols>
   <sheetData>
     <row r="1" ht="27.5">
-      <c r="A1" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
+      <c r="A1" s="90" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
     </row>
     <row r="2" ht="27.5">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="91"/>
-      <c r="M2" s="91"/>
-      <c r="N2" s="91"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="90"/>
+      <c r="N2" s="90"/>
     </row>
     <row r="3" ht="12" customHeight="1" s="3" customFormat="1">
       <c r="A3" s="14"/>
@@ -5805,57 +5900,57 @@
       <c r="L4" s="18"/>
       <c r="M4" s="4"/>
       <c r="N4" s="18" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" ht="25.4" customHeight="1">
-      <c r="A5" s="117" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="118" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="100" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="101"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="103" t="s">
+      <c r="A5" s="116" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="92"/>
+      <c r="C5" s="117" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="99" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="100"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="105"/>
+      <c r="N5" s="104"/>
     </row>
     <row r="6" ht="25.4" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="122" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="123"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="106"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="120"/>
+      <c r="J6" s="121" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="122"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="105"/>
     </row>
     <row r="7" ht="30" customHeight="1">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="70"/>
+      <c r="B7" s="69"/>
       <c r="C7" s="2"/>
       <c r="D7" s="7" t="s">
         <v>12</v>
@@ -5869,7 +5964,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="19"/>
@@ -5880,10 +5975,10 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" ht="21.5">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="72"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -6015,13 +6110,13 @@
       <c r="N16" s="39"/>
     </row>
     <row r="17" ht="24.9" customHeight="1" s="18" customFormat="1">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="83"/>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="84"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
       <c r="F17" s="35" t="s">
         <v>28</v>
       </c>
@@ -6031,14 +6126,14 @@
       <c r="H17" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="80" t="s">
+      <c r="I17" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="81"/>
-      <c r="K17" s="85" t="s">
+      <c r="J17" s="80"/>
+      <c r="K17" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="84"/>
+      <c r="L17" s="83"/>
       <c r="M17" s="40" t="s">
         <v>33</v>
       </c>
@@ -6048,107 +6143,107 @@
     </row>
     <row r="18" ht="24.9" customHeight="1" s="8" customFormat="1">
       <c r="A18" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="87"/>
+        <v>75</v>
+      </c>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="86"/>
       <c r="F18" s="31"/>
       <c r="G18" s="30"/>
       <c r="H18" s="44"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="89"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="87"/>
+      <c r="L18" s="88"/>
       <c r="M18" s="46"/>
       <c r="N18" s="50"/>
     </row>
     <row r="19" ht="24.9" customHeight="1" s="8" customFormat="1">
       <c r="A19" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="87"/>
+        <v>76</v>
+      </c>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="86"/>
       <c r="F19" s="31"/>
       <c r="G19" s="30"/>
       <c r="H19" s="44"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="88"/>
-      <c r="L19" s="89"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="88"/>
       <c r="M19" s="46"/>
       <c r="N19" s="51"/>
     </row>
     <row r="20" ht="24.9" customHeight="1" s="8" customFormat="1">
       <c r="A20" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
+        <v>77</v>
+      </c>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="86"/>
       <c r="F20" s="31"/>
       <c r="G20" s="30"/>
       <c r="H20" s="44"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="89"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="88"/>
       <c r="M20" s="46"/>
       <c r="N20" s="51"/>
     </row>
     <row r="21" ht="24.9" customHeight="1" s="8" customFormat="1">
-      <c r="A21" s="110" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="111"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="112"/>
+      <c r="A21" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="110"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="111"/>
       <c r="F21" s="29"/>
       <c r="G21" s="37"/>
       <c r="H21" s="45"/>
-      <c r="I21" s="113"/>
-      <c r="J21" s="114"/>
-      <c r="K21" s="115"/>
-      <c r="L21" s="116"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="115"/>
       <c r="M21" s="47"/>
       <c r="N21" s="52"/>
     </row>
     <row r="22" ht="68.4" customHeight="1" s="8" customFormat="1">
       <c r="A22" s="41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
       <c r="G22" s="43" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H22" s="23"/>
       <c r="I22" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="M22" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N22" s="26"/>
     </row>
     <row r="23" ht="24.75" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>